<commit_message>
Ajout de quelques composants
</commit_message>
<xml_diff>
--- a/Liste du matériel.xlsx
+++ b/Liste du matériel.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Partie</t>
   </si>
   <si>
-    <t>Composant</t>
-  </si>
-  <si>
     <t>Prix unit.</t>
   </si>
   <si>
@@ -79,7 +76,25 @@
     <t>KAPshop</t>
   </si>
   <si>
-    <t>?</t>
+    <t>Composants</t>
+  </si>
+  <si>
+    <t>Potentiomètre 10K</t>
+  </si>
+  <si>
+    <t>https://www.gotronic.fr/art-ajustable-horizontal-10k-8486-117.htm</t>
+  </si>
+  <si>
+    <t>Gotronic</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Led rouge</t>
+  </si>
+  <si>
+    <t>https://www.gotronic.fr/art-led-5mm-rouge-l51hd-2069.htm</t>
   </si>
 </sst>
 </file>
@@ -88,8 +103,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00\ [$€-80C]_-;\-* #,##0.00\ [$€-80C]_-;_-* &quot;-&quot;??\ [$€-80C]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-80C]_-;\-* #,##0.00\ [$€-80C]_-;_-* &quot;-&quot;??\ [$€-80C]_-;_-@_-"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -128,8 +143,8 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -436,16 +451,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J8"/>
+  <dimension ref="B2:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" customWidth="1"/>
     <col min="9" max="9" width="14.5546875" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
   </cols>
@@ -455,33 +471,33 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1">
         <v>20.75</v>
@@ -494,16 +510,16 @@
         <v>20.75</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
@@ -511,7 +527,7 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1">
         <v>7.57</v>
@@ -520,25 +536,25 @@
         <v>1</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" ref="F5:F6" si="0">D6*E6</f>
+        <f t="shared" ref="F6" si="0">D6*E6</f>
         <v>7.57</v>
       </c>
       <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="4">
         <v>4.75</v>
@@ -551,19 +567,84 @@
         <v>4.75</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="I8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>13</v>
+      <c r="D10" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" ref="F9:F12" si="1">D10*E10</f>
+        <v>0.5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="str">
+        <f>"04601"</f>
+        <v>04601</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" t="str">
+        <f>"03030"</f>
+        <v>03030</v>
+      </c>
+      <c r="I12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I10" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalisation de la liste des composants
</commit_message>
<xml_diff>
--- a/Liste du matériel.xlsx
+++ b/Liste du matériel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
   <si>
     <t>Partie</t>
   </si>
@@ -95,21 +95,135 @@
   </si>
   <si>
     <t>https://www.gotronic.fr/art-led-5mm-rouge-l51hd-2069.htm</t>
+  </si>
+  <si>
+    <t>Câble mâle-mâle</t>
+  </si>
+  <si>
+    <t>RS Components</t>
+  </si>
+  <si>
+    <t>791-6463</t>
+  </si>
+  <si>
+    <t>Câble mâle-femelle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">791-6454 </t>
+  </si>
+  <si>
+    <t>https://befr.rs-online.com/web/p/breadboard-jumper-wire-kits/7916454/</t>
+  </si>
+  <si>
+    <t>https://befr.rs-online.com/web/p/breadboard-jumper-wire-kits/7916463/?sra=pstk</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 3 B+</t>
+  </si>
+  <si>
+    <t>174-7510</t>
+  </si>
+  <si>
+    <t>https://befr.rs-online.com/web/p/processor-microcontroller-development-kits/1747510/</t>
+  </si>
+  <si>
+    <t>Pi caméra V2</t>
+  </si>
+  <si>
+    <t>913-2664</t>
+  </si>
+  <si>
+    <t>https://befr.rs-online.com/web/p/video-modules/9132664/</t>
+  </si>
+  <si>
+    <t>Arduino</t>
+  </si>
+  <si>
+    <t>Raspberry</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Résistance 220ohms Pack de 10</t>
+  </si>
+  <si>
+    <t>135-500</t>
+  </si>
+  <si>
+    <t>https://befr.rs-online.com/web/p/through-hole-fixed-resistors/0135500/</t>
+  </si>
+  <si>
+    <t>Jumper Cable Kit Fil</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/SODIAL-140pcs-essais-soudure-Arduino/dp/B00K67XXSI/ref=pd_rhf_se_s_cr_simh_0_2/258-3828012-1800823?_encoding=UTF8&amp;pd_rd_i=B00K67XXSI&amp;pd_rd_r=ee7e71c4-6cc0-4d52-905a-c4d2313b0ed9&amp;pd_rd_w=IK5Hy&amp;pd_rd_wg=E01pP&amp;pf_rd_p=6a290ea9-6266-4603-ae1c-ee92d8380ae8&amp;pf_rd_r=WKSH6W7DKZCYSTSY9X40&amp;psc=1&amp;refRID=WKSH6W7DKZCYSTSY9X40</t>
+  </si>
+  <si>
+    <t>Bois</t>
+  </si>
+  <si>
+    <t>Récupération</t>
+  </si>
+  <si>
+    <t>Impression 3D</t>
+  </si>
+  <si>
+    <t>Barrière</t>
+  </si>
+  <si>
+    <t>( m )</t>
+  </si>
+  <si>
+    <t>( g )</t>
+  </si>
+  <si>
+    <t>Prix total</t>
+  </si>
+  <si>
+    <t>Support haut du servo</t>
+  </si>
+  <si>
+    <t>Support bas du servo</t>
+  </si>
+  <si>
+    <t>Nombre d'essai</t>
+  </si>
+  <si>
+    <t>Montage pratique</t>
+  </si>
+  <si>
+    <t>( €/g )</t>
+  </si>
+  <si>
+    <t>Sous-total</t>
+  </si>
+  <si>
+    <t>Total général</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="6">
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-80C]_-;\-* #,##0.00\ [$€-80C]_-;_-* &quot;-&quot;??\ [$€-80C]_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -137,16 +251,446 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,200 +995,713 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J12"/>
+  <dimension ref="B1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.109375" customWidth="1"/>
     <col min="9" max="9" width="14.5546875" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="47">
         <v>20.75</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="17">
         <v>1</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="18">
         <f>D4*E4</f>
         <v>20.75</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F5" s="2"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="49">
         <v>7.57</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="21">
         <v>1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="22">
         <f t="shared" ref="F6" si="0">D6*E6</f>
         <v>7.57</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="24" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="5"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="23"/>
+    </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="50">
         <v>4.75</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="21">
         <v>1</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="25">
         <f>D8*E8</f>
         <v>4.75</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="24" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="23"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="50">
         <v>0.25</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="21">
         <v>2</v>
       </c>
-      <c r="F10" s="4">
-        <f t="shared" ref="F9:F12" si="1">D10*E10</f>
+      <c r="F10" s="25">
+        <f t="shared" ref="F10:F14" si="1">D10*E10</f>
         <v>0.5</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="H10" t="str">
+      <c r="H10" s="21" t="str">
         <f>"04601"</f>
         <v>04601</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="24" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="23"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="50">
         <v>0.15</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4">
+      <c r="E12" s="21">
+        <v>2</v>
+      </c>
+      <c r="F12" s="25">
         <f t="shared" si="1"/>
-        <v>0.15</v>
-      </c>
-      <c r="G12" t="s">
+        <v>0.3</v>
+      </c>
+      <c r="G12" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="H12" t="str">
+      <c r="H12" s="21" t="str">
         <f>"03030"</f>
         <v>03030</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="24" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="5"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="23"/>
+    </row>
+    <row r="14" spans="2:10" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="6"/>
+      <c r="C14" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="55">
+        <v>0.26</v>
+      </c>
+      <c r="E14" s="27">
+        <v>1</v>
+      </c>
+      <c r="F14" s="28">
+        <f t="shared" si="1"/>
+        <v>0.26</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="31"/>
+      <c r="C15" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="54">
+        <f>SUM(D4:D14)</f>
+        <v>33.729999999999997</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="33"/>
+    </row>
+    <row r="16" spans="2:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="56">
+        <v>63.7</v>
+      </c>
+      <c r="E16" s="17">
+        <v>1</v>
+      </c>
+      <c r="F16" s="34">
+        <f>D16*E16</f>
+        <v>63.7</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="23"/>
+    </row>
+    <row r="18" spans="2:10" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="3"/>
+      <c r="C18" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="55">
+        <v>23.09</v>
+      </c>
+      <c r="E18" s="36">
+        <v>1</v>
+      </c>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="38"/>
+      <c r="C19" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="54">
+        <f>SUM(D16:D18)</f>
+        <v>86.79</v>
+      </c>
+      <c r="E19" s="39"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="41"/>
+    </row>
+    <row r="20" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="51">
+        <v>2.41</v>
+      </c>
+      <c r="E20" s="17">
+        <v>1</v>
+      </c>
+      <c r="F20" s="34">
+        <f>D20*E20</f>
+        <v>2.41</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="8"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="23"/>
+    </row>
+    <row r="22" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="8"/>
+      <c r="C22" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="50">
+        <v>2.41</v>
+      </c>
+      <c r="E22" s="21">
+        <v>2</v>
+      </c>
+      <c r="F22" s="25">
+        <f>D22*E22</f>
+        <v>4.82</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="8"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="23"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="9"/>
+      <c r="C24" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="52">
+        <v>2.5</v>
+      </c>
+      <c r="E24" s="36">
+        <v>1</v>
+      </c>
+      <c r="F24" s="42">
+        <f t="shared" ref="F24" si="2">D24*E24</f>
+        <v>2.5</v>
+      </c>
+      <c r="G24" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="43">
+        <v>14731</v>
+      </c>
+      <c r="I24" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="J24" s="37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="38"/>
+      <c r="C25" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="54">
+        <f>SUM(D20:D24)</f>
+        <v>7.32</v>
+      </c>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="41"/>
+    </row>
+    <row r="26" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="53">
+        <v>20</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="5"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="23"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="5"/>
+      <c r="C28" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" s="15"/>
+      <c r="J28" s="46"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="5"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="23"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="5"/>
+      <c r="C30" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="21">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E30" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="F30" s="21">
+        <v>6</v>
+      </c>
+      <c r="G30" s="21">
+        <v>2</v>
+      </c>
+      <c r="H30" s="59">
+        <f>D30*F30*G30</f>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="I30" s="21"/>
+      <c r="J30" s="45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="5"/>
+      <c r="C31" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="21">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E31" s="21">
+        <v>0.49</v>
+      </c>
+      <c r="F31" s="21">
+        <v>3</v>
+      </c>
+      <c r="G31" s="21">
+        <v>1</v>
+      </c>
+      <c r="H31" s="59">
+        <f>D31*F31*G31</f>
+        <v>0.10500000000000001</v>
+      </c>
+      <c r="I31" s="21"/>
+      <c r="J31" s="45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="5"/>
+      <c r="C32" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="21">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E32" s="21">
+        <v>1.2</v>
+      </c>
+      <c r="F32" s="21">
+        <v>8</v>
+      </c>
+      <c r="G32" s="21">
+        <v>1</v>
+      </c>
+      <c r="H32" s="59">
+        <f>D32*F32*G32</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I32" s="21"/>
+      <c r="J32" s="45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="31"/>
+      <c r="C33" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="63">
+        <f>SUM(H29:H32)</f>
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="I33" s="32"/>
+      <c r="J33" s="33"/>
+    </row>
+    <row r="34" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="60"/>
+      <c r="C34" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="65">
+        <f>SUM(D15,D19,D25,H33)</f>
+        <v>128.64500000000001</v>
+      </c>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="62"/>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I10" r:id="rId1"/>
-  </hyperlinks>
+  <mergeCells count="13">
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B4:B14"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B26:B32"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>